<commit_message>
Agregado el modelo de ingresos, primer borrador.
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Presupuesto/Presupuesto pickupmeal.xlsx
+++ b/SAP - NEGOCIO/Temporal/Presupuesto/Presupuesto pickupmeal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\SAP-TFI 2015\sap-tfi-documentation\SAP - NEGOCIO\Temporal\Presupuesto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,6 +17,9 @@
     <sheet name="Inversion Inicial P2" sheetId="3" r:id="rId3"/>
     <sheet name="Costos Fijos P2" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
@@ -343,51 +346,61 @@
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF9900"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -468,16 +481,44 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -754,7 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -770,11 +811,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
+      <c r="A1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -996,7 +1037,7 @@
       <c r="E9" s="6">
         <v>90000</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="26" t="s">
         <v>97</v>
       </c>
       <c r="P9" s="3"/>
@@ -1160,7 +1201,7 @@
       <c r="E15" s="25">
         <v>99500</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="26" t="s">
         <v>98</v>
       </c>
       <c r="G15" s="3"/>
@@ -1191,7 +1232,7 @@
       <c r="E16" s="25">
         <v>1500</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="26" t="s">
         <v>99</v>
       </c>
       <c r="G16" s="3"/>
@@ -1508,7 +1549,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2035,7 +2076,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2044,11 +2087,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
+      <c r="A1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
@@ -2380,15 +2423,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2456,7 +2501,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Actualización presupuesto y Punto 2.2.4
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Presupuesto/Presupuesto pickupmeal.xlsx
+++ b/SAP - NEGOCIO/Temporal/Presupuesto/Presupuesto pickupmeal.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\SAP-TFI 2015\sap-tfi-documentation\SAP - NEGOCIO\Temporal\Presupuesto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\SAPgit\sap-tfi-documentation\SAP - NEGOCIO\Temporal\Presupuesto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inversión inicial P1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="115">
   <si>
     <t>Recursos</t>
   </si>
@@ -325,13 +325,59 @@
   </si>
   <si>
     <t>http://articulo.mercadolibre.com.ar/MLA-578884349-casco-abierto-vertigo-basic-negro-obviamente-en-fas-motos-_JM</t>
+  </si>
+  <si>
+    <t>Ingeniero de Software</t>
+  </si>
+  <si>
+    <t>Neto</t>
+  </si>
+  <si>
+    <t>Desarrollador semiSenior</t>
+  </si>
+  <si>
+    <t>Lider de desarrollo semiSenior</t>
+  </si>
+  <si>
+    <t>Extras</t>
+  </si>
+  <si>
+    <t>Fuente: ar.indeed.com</t>
+  </si>
+  <si>
+    <t>Servicio VPN para el sitio web, en la página donweb.com. Precio por año</t>
+  </si>
+  <si>
+    <t>insumo</t>
+  </si>
+  <si>
+    <t>Repositorio</t>
+  </si>
+  <si>
+    <t>Cuenta privada de github</t>
+  </si>
+  <si>
+    <t>Servicio de conexión a Internet, Fibercorp dinámico 10M-1M</t>
+  </si>
+  <si>
+    <t>Ingeniero Logística</t>
+  </si>
+  <si>
+    <t>Lider de logística</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Lider de marketing junior</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]&quot;$&quot;\ \-#,##0"/>
     <numFmt numFmtId="164" formatCode="\$#,##0"/>
     <numFmt numFmtId="165" formatCode="[$$-2C0A]#,##0.00;[Red]\([$$-2C0A]#,##0.00\)"/>
   </numFmts>
@@ -417,7 +463,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -425,12 +471,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -465,9 +526,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -482,8 +540,27 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1013,7 +1090,7 @@
       <c r="E8" s="6">
         <v>15115</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="20" t="s">
         <v>40</v>
       </c>
       <c r="G8" s="4"/>
@@ -1037,7 +1114,7 @@
       <c r="E9" s="6">
         <v>90000</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="25" t="s">
         <v>97</v>
       </c>
       <c r="P9" s="3"/>
@@ -1059,7 +1136,7 @@
       <c r="E10" s="6">
         <v>3600</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="20" t="s">
         <v>74</v>
       </c>
       <c r="P10" s="3"/>
@@ -1081,7 +1158,7 @@
       <c r="E11" s="6">
         <v>738</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="20" t="s">
         <v>75</v>
       </c>
       <c r="I11" s="3"/>
@@ -1104,7 +1181,7 @@
       <c r="C12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="17">
@@ -1170,7 +1247,7 @@
       <c r="E14" s="17">
         <v>750</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="23" t="s">
         <v>80</v>
       </c>
       <c r="G14" s="3"/>
@@ -1198,10 +1275,10 @@
       <c r="D15" s="12">
         <v>5</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="24">
         <v>99500</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="25" t="s">
         <v>98</v>
       </c>
       <c r="G15" s="3"/>
@@ -1229,10 +1306,10 @@
       <c r="D16" s="12">
         <v>5</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="24">
         <v>1500</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="25" t="s">
         <v>99</v>
       </c>
       <c r="G16" s="3"/>
@@ -1260,7 +1337,7 @@
       <c r="D17" s="12">
         <v>5</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="24">
         <v>1500</v>
       </c>
       <c r="F17" s="12"/>
@@ -1292,7 +1369,7 @@
       <c r="E18" s="17">
         <v>1500</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="23" t="s">
         <v>89</v>
       </c>
       <c r="G18" s="3"/>
@@ -1323,7 +1400,7 @@
       <c r="E19" s="17">
         <v>5300</v>
       </c>
-      <c r="F19" s="24"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1378,7 +1455,7 @@
       <c r="D21" s="3">
         <v>5</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="21">
         <v>5000</v>
       </c>
       <c r="F21" s="3"/>
@@ -1407,7 +1484,7 @@
       <c r="D22" s="3">
         <v>1</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="21">
         <v>1000</v>
       </c>
       <c r="F22" s="3"/>
@@ -1436,7 +1513,7 @@
       <c r="D23" s="3">
         <v>1</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="21">
         <v>5000</v>
       </c>
       <c r="F23" s="3"/>
@@ -1546,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1559,7 +1636,9 @@
     <col min="3" max="3" width="49.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="15" width="13.7109375" customWidth="1"/>
+    <col min="6" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="15" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1578,8 +1657,12 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -1607,20 +1690,20 @@
       <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="18">
-        <v>3000</v>
+      <c r="B3" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="32">
+        <v>1</v>
+      </c>
+      <c r="E3" s="34">
+        <v>10000</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1634,22 +1717,25 @@
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6">
-        <v>3000</v>
-      </c>
-      <c r="F4" s="3"/>
+      <c r="B4" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="32">
+        <v>3</v>
+      </c>
+      <c r="E4" s="34">
+        <f>F4*3</f>
+        <v>18651</v>
+      </c>
+      <c r="F4" s="3">
+        <v>6217</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1661,209 +1747,206 @@
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="4">
-        <v>3</v>
-      </c>
-      <c r="E5" s="6">
-        <v>2500</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
+      <c r="B5" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="32">
+        <v>1</v>
+      </c>
+      <c r="E5" s="34">
+        <v>4500</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
     </row>
     <row r="6" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6">
-        <v>3500</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-    </row>
-    <row r="7" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="B6" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="32">
+        <v>1</v>
+      </c>
+      <c r="E6" s="34">
+        <v>4500</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6">
-        <v>3500</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="32">
+        <v>1</v>
+      </c>
+      <c r="E7" s="34">
+        <f>F7+G7</f>
+        <v>17545</v>
+      </c>
+      <c r="F7" s="30">
+        <v>15125</v>
+      </c>
+      <c r="G7" s="12">
+        <f>F7*0.16</f>
+        <v>2420</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+    </row>
+    <row r="8" spans="1:15" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="32">
+        <v>1</v>
+      </c>
+      <c r="E8" s="35">
+        <f>F8+G8</f>
+        <v>17545</v>
+      </c>
+      <c r="F8" s="6">
+        <v>15125</v>
+      </c>
+      <c r="G8" s="12">
+        <f>F7*0.16</f>
+        <v>2420</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="36">
+        <v>1</v>
+      </c>
+      <c r="E9" s="37">
+        <f>F9+H9</f>
+        <v>18425</v>
+      </c>
+      <c r="F9">
+        <v>18425</v>
+      </c>
+      <c r="G9">
+        <f>F9*0.3</f>
+        <v>5527.5</v>
+      </c>
+      <c r="J9" s="29"/>
+    </row>
+    <row r="10" spans="1:15" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="36">
+        <v>1</v>
+      </c>
+      <c r="E10" s="37">
+        <v>14668</v>
+      </c>
+      <c r="J10" s="29"/>
+    </row>
+    <row r="11" spans="1:15" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="36">
+        <v>1</v>
+      </c>
+      <c r="E11" s="37">
+        <v>12900</v>
+      </c>
+      <c r="J11" s="29"/>
+    </row>
+    <row r="12" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B12" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="12">
-        <v>2</v>
-      </c>
-      <c r="E9" s="17">
-        <v>2000</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="12">
-        <v>1</v>
-      </c>
-      <c r="E10" s="17">
-        <v>550</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="17">
-        <v>500</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="17">
-        <v>900</v>
+      <c r="C12" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="32">
+        <v>1</v>
+      </c>
+      <c r="E12" s="31">
+        <v>1944</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1876,44 +1959,48 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3">
-        <v>300</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+    <row r="13" spans="1:15" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="32">
+        <v>1</v>
+      </c>
+      <c r="E13" s="31">
+        <v>250</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
     </row>
     <row r="14" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="12">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3">
-        <v>2500</v>
+      <c r="A14" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="38">
+        <v>1</v>
+      </c>
+      <c r="E14" s="40">
+        <v>2000</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1926,12 +2013,22 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+    <row r="15" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="38">
+        <v>1</v>
+      </c>
+      <c r="E15" s="40">
+        <v>848</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1944,15 +2041,20 @@
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="17">
-        <f>SUM(E3:E14)</f>
-        <v>22250</v>
+      <c r="A16" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="40">
+        <v>500</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1966,11 +2068,21 @@
       <c r="O16" s="3"/>
     </row>
     <row r="17" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="A17" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="38">
+        <v>1</v>
+      </c>
+      <c r="E17" s="40">
+        <v>900</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1983,11 +2095,17 @@
       <c r="O17" s="3"/>
     </row>
     <row r="18" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="A18" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38">
+        <v>300</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -2000,11 +2118,21 @@
       <c r="O18" s="3"/>
     </row>
     <row r="19" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="A19" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="38">
+        <v>1</v>
+      </c>
+      <c r="E19" s="38">
+        <v>2500</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2017,11 +2145,11 @@
       <c r="O19" s="3"/>
     </row>
     <row r="20" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -2034,11 +2162,16 @@
       <c r="O20" s="3"/>
     </row>
     <row r="21" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="40">
+        <f>SUM(E3:E19)</f>
+        <v>127976</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -2067,8 +2200,94 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
     </row>
+    <row r="23" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2268,7 +2487,7 @@
       <c r="C12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="17">
@@ -2339,7 +2558,7 @@
       <c r="D16" s="3">
         <v>1</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="21">
         <v>1000</v>
       </c>
     </row>
@@ -2356,41 +2575,41 @@
       <c r="D17" s="3">
         <v>1</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="21">
         <v>5000</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="19">
-        <v>1</v>
-      </c>
-      <c r="E18" s="19">
+      <c r="D18" s="18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="18">
         <v>35000</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="19">
+      <c r="D19" s="18">
+        <v>1</v>
+      </c>
+      <c r="E19" s="18">
         <v>8790</v>
       </c>
     </row>
@@ -2570,19 +2789,19 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="19">
-        <v>1</v>
-      </c>
-      <c r="E9" s="19">
+      <c r="D9" s="18">
+        <v>1</v>
+      </c>
+      <c r="E9" s="18">
         <v>3000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Falta cadena de valor
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Presupuesto/Presupuesto pickupmeal.xlsx
+++ b/SAP - NEGOCIO/Temporal/Presupuesto/Presupuesto pickupmeal.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inversión inicial P1" sheetId="1" r:id="rId1"/>
@@ -541,8 +541,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="6" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -561,6 +559,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -888,11 +888,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="A1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -1626,7 +1626,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1690,19 +1690,19 @@
       <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="32">
-        <v>1</v>
-      </c>
-      <c r="E3" s="34">
+      <c r="D3" s="30">
+        <v>1</v>
+      </c>
+      <c r="E3" s="32">
         <v>10000</v>
       </c>
       <c r="F3" s="3"/>
@@ -1717,21 +1717,21 @@
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="32">
-        <v>3</v>
-      </c>
-      <c r="E4" s="34">
-        <f>F4*3</f>
-        <v>18651</v>
+      <c r="D4" s="30">
+        <v>5</v>
+      </c>
+      <c r="E4" s="32">
+        <f>F4*5</f>
+        <v>31085</v>
       </c>
       <c r="F4" s="3">
         <v>6217</v>
@@ -1747,19 +1747,19 @@
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="32">
-        <v>1</v>
-      </c>
-      <c r="E5" s="34">
+      <c r="D5" s="30">
+        <v>1</v>
+      </c>
+      <c r="E5" s="32">
         <v>4500</v>
       </c>
       <c r="F5" s="12"/>
@@ -1776,19 +1776,19 @@
       <c r="O5" s="12"/>
     </row>
     <row r="6" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="32">
-        <v>1</v>
-      </c>
-      <c r="E6" s="34">
+      <c r="D6" s="30">
+        <v>1</v>
+      </c>
+      <c r="E6" s="32">
         <v>4500</v>
       </c>
       <c r="F6" s="3"/>
@@ -1805,23 +1805,23 @@
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="32">
-        <v>1</v>
-      </c>
-      <c r="E7" s="34">
+      <c r="D7" s="30">
+        <v>1</v>
+      </c>
+      <c r="E7" s="32">
         <f>F7+G7</f>
         <v>17545</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="28">
         <v>15125</v>
       </c>
       <c r="G7" s="12">
@@ -1838,19 +1838,19 @@
       <c r="O7" s="12"/>
     </row>
     <row r="8" spans="1:15" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="32">
-        <v>1</v>
-      </c>
-      <c r="E8" s="35">
+      <c r="D8" s="30">
+        <v>1</v>
+      </c>
+      <c r="E8" s="33">
         <f>F8+G8</f>
         <v>17545</v>
       </c>
@@ -1871,19 +1871,19 @@
       <c r="O8" s="12"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="36">
-        <v>1</v>
-      </c>
-      <c r="E9" s="37">
+      <c r="D9" s="34">
+        <v>1</v>
+      </c>
+      <c r="E9" s="35">
         <f>F9+H9</f>
         <v>18425</v>
       </c>
@@ -1894,58 +1894,58 @@
         <f>F9*0.3</f>
         <v>5527.5</v>
       </c>
-      <c r="J9" s="29"/>
+      <c r="J9" s="27"/>
     </row>
     <row r="10" spans="1:15" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="36">
-        <v>1</v>
-      </c>
-      <c r="E10" s="37">
+      <c r="D10" s="34">
+        <v>1</v>
+      </c>
+      <c r="E10" s="35">
         <v>14668</v>
       </c>
-      <c r="J10" s="29"/>
+      <c r="J10" s="27"/>
     </row>
     <row r="11" spans="1:15" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="36">
-        <v>1</v>
-      </c>
-      <c r="E11" s="37">
+      <c r="D11" s="34">
+        <v>1</v>
+      </c>
+      <c r="E11" s="35">
         <v>12900</v>
       </c>
-      <c r="J11" s="29"/>
+      <c r="J11" s="27"/>
     </row>
     <row r="12" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="32">
-        <v>1</v>
-      </c>
-      <c r="E12" s="31">
+      <c r="D12" s="30">
+        <v>1</v>
+      </c>
+      <c r="E12" s="29">
         <v>1944</v>
       </c>
       <c r="F12" s="3"/>
@@ -1960,19 +1960,19 @@
       <c r="O12" s="3"/>
     </row>
     <row r="13" spans="1:15" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="32">
-        <v>1</v>
-      </c>
-      <c r="E13" s="31">
+      <c r="D13" s="30">
+        <v>1</v>
+      </c>
+      <c r="E13" s="29">
         <v>250</v>
       </c>
       <c r="F13" s="12"/>
@@ -1987,19 +1987,19 @@
       <c r="O13" s="12"/>
     </row>
     <row r="14" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="38">
-        <v>1</v>
-      </c>
-      <c r="E14" s="40">
+      <c r="D14" s="36">
+        <v>1</v>
+      </c>
+      <c r="E14" s="38">
         <v>2000</v>
       </c>
       <c r="F14" s="3"/>
@@ -2014,19 +2014,19 @@
       <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="D15" s="38">
-        <v>1</v>
-      </c>
-      <c r="E15" s="40">
+      <c r="D15" s="36">
+        <v>1</v>
+      </c>
+      <c r="E15" s="38">
         <v>848</v>
       </c>
       <c r="F15" s="3"/>
@@ -2041,19 +2041,19 @@
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="40">
+      <c r="E16" s="38">
         <v>500</v>
       </c>
       <c r="F16" s="3"/>
@@ -2068,19 +2068,19 @@
       <c r="O16" s="3"/>
     </row>
     <row r="17" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="38">
-        <v>1</v>
-      </c>
-      <c r="E17" s="40">
+      <c r="D17" s="36">
+        <v>1</v>
+      </c>
+      <c r="E17" s="38">
         <v>900</v>
       </c>
       <c r="F17" s="3"/>
@@ -2095,15 +2095,15 @@
       <c r="O17" s="3"/>
     </row>
     <row r="18" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38">
+      <c r="C18" s="37"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36">
         <v>300</v>
       </c>
       <c r="F18" s="3"/>
@@ -2118,20 +2118,20 @@
       <c r="O18" s="3"/>
     </row>
     <row r="19" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="38">
-        <v>1</v>
-      </c>
-      <c r="E19" s="38">
-        <v>2500</v>
+      <c r="D19" s="36">
+        <v>1</v>
+      </c>
+      <c r="E19" s="36">
+        <v>6000</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -2145,11 +2145,11 @@
       <c r="O19" s="3"/>
     </row>
     <row r="20" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -2162,15 +2162,15 @@
       <c r="O20" s="3"/>
     </row>
     <row r="21" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="38"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38" t="s">
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="40">
+      <c r="E21" s="38">
         <f>SUM(E3:E19)</f>
-        <v>127976</v>
+        <v>143910</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -2306,11 +2306,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="A1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>

</xml_diff>